<commit_message>
Build explanation text; Update progress tracker
</commit_message>
<xml_diff>
--- a/C_Output/best_month_for_route.xlsx
+++ b/C_Output/best_month_for_route.xlsx
@@ -473,14 +473,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Missouri Plus</t>
+          <t>Louisiana Plus</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="C2" t="n">
-        <v>0.72</v>
+        <v>0.74</v>
       </c>
       <c r="D2" t="n">
         <v>0.72</v>
@@ -493,24 +493,24 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>05-27</t>
+          <t>04-07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Missouri Plus</t>
+          <t>Louisiana Plus</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>282</v>
+        <v>337</v>
       </c>
       <c r="C3" t="n">
-        <v>0.74</v>
+        <v>0.68</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.67</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -520,24 +520,24 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>10-09</t>
+          <t>12-03</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Puerto Rico</t>
+          <t>Near DC</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1</v>
+        <v>0.71</v>
       </c>
       <c r="D4" t="n">
-        <v>0.08</v>
+        <v>0.74</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -547,24 +547,24 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>03-08</t>
+          <t>05-17</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Puerto Rico</t>
+          <t>Near DC</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>365</v>
+        <v>297</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05</v>
+        <v>0.77</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02</v>
+        <v>0.79</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -574,24 +574,24 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>12-31</t>
+          <t>10-24</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Northeast Plus</t>
+          <t>Oregon Plus</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C6" t="n">
         <v>0.74</v>
       </c>
       <c r="D6" t="n">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -601,24 +601,24 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>06-06</t>
+          <t>06-26</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Northeast Plus</t>
+          <t>Oregon Plus</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="C7" t="n">
-        <v>0.78</v>
+        <v>0.82</v>
       </c>
       <c r="D7" t="n">
-        <v>0.77</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -628,24 +628,24 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>10-14</t>
+          <t>09-29</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>New Mexico Plus</t>
+          <t>Northeast Plus</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>107</v>
+        <v>157</v>
       </c>
       <c r="C8" t="n">
-        <v>0.59</v>
+        <v>0.74</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6</v>
+        <v>0.72</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -655,24 +655,24 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>04-17</t>
+          <t>06-06</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>New Mexico Plus</t>
+          <t>Northeast Plus</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6</v>
+        <v>0.78</v>
       </c>
       <c r="D9" t="n">
-        <v>0.59</v>
+        <v>0.77</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -682,24 +682,24 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>10-24</t>
+          <t>10-14</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Indiana Plus</t>
+          <t>Minnesota Plus</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C10" t="n">
-        <v>0.76</v>
+        <v>0.8</v>
       </c>
       <c r="D10" t="n">
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -709,24 +709,24 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>06-06</t>
+          <t>06-26</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Indiana Plus</t>
+          <t>Minnesota Plus</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C11" t="n">
-        <v>0.73</v>
+        <v>0.77</v>
       </c>
       <c r="D11" t="n">
-        <v>0.75</v>
+        <v>0.77</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -736,24 +736,24 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>09-19</t>
+          <t>09-09</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Wyoming Plus</t>
+          <t>Hawaii State</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>157</v>
+        <v>52</v>
       </c>
       <c r="C12" t="n">
-        <v>0.66</v>
+        <v>0.76</v>
       </c>
       <c r="D12" t="n">
-        <v>0.65</v>
+        <v>0.79</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -763,24 +763,24 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>06-06</t>
+          <t>02-21</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Wyoming Plus</t>
+          <t>Hawaii State</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>272</v>
+        <v>365</v>
       </c>
       <c r="C13" t="n">
-        <v>0.61</v>
+        <v>0.64</v>
       </c>
       <c r="D13" t="n">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -790,24 +790,24 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>09-29</t>
+          <t>12-31</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Near DC</t>
+          <t>Alaska State</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="C14" t="n">
-        <v>0.71</v>
+        <v>0.85</v>
       </c>
       <c r="D14" t="n">
-        <v>0.74</v>
+        <v>0.88</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -817,24 +817,24 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>05-17</t>
+          <t>07-19</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Near DC</t>
+          <t>Alaska State</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>297</v>
+        <v>246</v>
       </c>
       <c r="C15" t="n">
-        <v>0.77</v>
+        <v>0.87</v>
       </c>
       <c r="D15" t="n">
-        <v>0.79</v>
+        <v>0.87</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -844,24 +844,24 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>10-24</t>
+          <t>09-03</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Louisiana Plus</t>
+          <t>Wyoming Plus</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>97</v>
+        <v>157</v>
       </c>
       <c r="C16" t="n">
-        <v>0.74</v>
+        <v>0.66</v>
       </c>
       <c r="D16" t="n">
-        <v>0.72</v>
+        <v>0.65</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -871,24 +871,24 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>04-07</t>
+          <t>06-06</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Louisiana Plus</t>
+          <t>Wyoming Plus</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>337</v>
+        <v>272</v>
       </c>
       <c r="C17" t="n">
-        <v>0.68</v>
+        <v>0.61</v>
       </c>
       <c r="D17" t="n">
-        <v>0.67</v>
+        <v>0.62</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -898,24 +898,24 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>12-03</t>
+          <t>09-29</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>East Canada</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>182</v>
+        <v>37</v>
       </c>
       <c r="C18" t="n">
-        <v>0.77</v>
+        <v>0.71</v>
       </c>
       <c r="D18" t="n">
-        <v>0.77</v>
+        <v>0.7</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -925,24 +925,24 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>07-01</t>
+          <t>02-06</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>East Canada</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>257</v>
+        <v>362</v>
       </c>
       <c r="C19" t="n">
-        <v>0.78</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -952,24 +952,24 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>09-14</t>
+          <t>12-28</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Oregon Plus</t>
+          <t>Missouri Plus</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="C20" t="n">
-        <v>0.74</v>
+        <v>0.72</v>
       </c>
       <c r="D20" t="n">
-        <v>0.77</v>
+        <v>0.72</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -979,24 +979,24 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>06-26</t>
+          <t>05-27</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Oregon Plus</t>
+          <t>Missouri Plus</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="C21" t="n">
-        <v>0.82</v>
+        <v>0.74</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -1006,24 +1006,24 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>09-29</t>
+          <t>10-09</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Georgia Plus</t>
+          <t>Puerto Rico</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="C22" t="n">
-        <v>0.78</v>
+        <v>0.1</v>
       </c>
       <c r="D22" t="n">
-        <v>0.75</v>
+        <v>0.08</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1033,24 +1033,24 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>04-27</t>
+          <t>03-08</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Georgia Plus</t>
+          <t>Puerto Rico</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>302</v>
+        <v>365</v>
       </c>
       <c r="C23" t="n">
-        <v>0.74</v>
+        <v>0.05</v>
       </c>
       <c r="D23" t="n">
-        <v>0.75</v>
+        <v>0.02</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -1060,24 +1060,24 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>10-29</t>
+          <t>12-31</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Minnesota Plus</t>
+          <t>East Canada</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8</v>
+        <v>0.77</v>
       </c>
       <c r="D24" t="n">
-        <v>0.71</v>
+        <v>0.77</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1087,24 +1087,24 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>06-26</t>
+          <t>07-01</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Minnesota Plus</t>
+          <t>East Canada</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C25" t="n">
-        <v>0.77</v>
+        <v>0.78</v>
       </c>
       <c r="D25" t="n">
-        <v>0.77</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -1114,24 +1114,24 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>09-09</t>
+          <t>09-14</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Alaska State</t>
+          <t>California Plus</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>200</v>
+        <v>142</v>
       </c>
       <c r="C26" t="n">
-        <v>0.85</v>
+        <v>0.72</v>
       </c>
       <c r="D26" t="n">
-        <v>0.88</v>
+        <v>0.73</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1141,24 +1141,24 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>07-19</t>
+          <t>05-22</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Alaska State</t>
+          <t>California Plus</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>246</v>
+        <v>312</v>
       </c>
       <c r="C27" t="n">
-        <v>0.87</v>
+        <v>0.71</v>
       </c>
       <c r="D27" t="n">
-        <v>0.87</v>
+        <v>0.73</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -1168,24 +1168,24 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>09-03</t>
+          <t>11-08</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>California Plus</t>
+          <t>Georgia Plus</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="C28" t="n">
-        <v>0.72</v>
+        <v>0.78</v>
       </c>
       <c r="D28" t="n">
-        <v>0.73</v>
+        <v>0.75</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -1195,24 +1195,24 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>05-22</t>
+          <t>04-27</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>California Plus</t>
+          <t>Georgia Plus</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="C29" t="n">
-        <v>0.71</v>
+        <v>0.74</v>
       </c>
       <c r="D29" t="n">
-        <v>0.73</v>
+        <v>0.75</v>
       </c>
       <c r="E29" t="n">
         <v>1</v>
@@ -1222,24 +1222,24 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>11-08</t>
+          <t>10-29</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Indiana Plus</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>37</v>
+        <v>157</v>
       </c>
       <c r="C30" t="n">
-        <v>0.71</v>
+        <v>0.76</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -1249,24 +1249,24 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>02-06</t>
+          <t>06-06</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Indiana Plus</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>362</v>
+        <v>262</v>
       </c>
       <c r="C31" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.73</v>
       </c>
       <c r="D31" t="n">
-        <v>0.67</v>
+        <v>0.75</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
@@ -1276,24 +1276,24 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>12-28</t>
+          <t>09-19</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Hawaii State</t>
+          <t>New Mexico Plus</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="C32" t="n">
-        <v>0.76</v>
+        <v>0.59</v>
       </c>
       <c r="D32" t="n">
-        <v>0.79</v>
+        <v>0.6</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1303,24 +1303,24 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>02-21</t>
+          <t>04-17</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Hawaii State</t>
+          <t>New Mexico Plus</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>365</v>
+        <v>297</v>
       </c>
       <c r="C33" t="n">
-        <v>0.64</v>
+        <v>0.6</v>
       </c>
       <c r="D33" t="n">
-        <v>0.63</v>
+        <v>0.59</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>12-31</t>
+          <t>10-24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish test 1; improve code based on test 1 results
</commit_message>
<xml_diff>
--- a/C_Output/best_month_for_route.xlsx
+++ b/C_Output/best_month_for_route.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,17 +473,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Louisiana Plus</t>
+          <t>East Canada</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>97</v>
+        <v>177</v>
       </c>
       <c r="C2" t="n">
-        <v>0.74</v>
+        <v>0.84</v>
       </c>
       <c r="D2" t="n">
-        <v>0.72</v>
+        <v>0.82</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -493,24 +493,24 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>04-07</t>
+          <t>06-26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Louisiana Plus</t>
+          <t>East Canada</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>337</v>
+        <v>257</v>
       </c>
       <c r="C3" t="n">
-        <v>0.68</v>
+        <v>0.86</v>
       </c>
       <c r="D3" t="n">
-        <v>0.67</v>
+        <v>0.86</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -520,24 +520,24 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>12-03</t>
+          <t>09-14</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Near DC</t>
+          <t>Wyoming Plus</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C4" t="n">
         <v>0.71</v>
       </c>
       <c r="D4" t="n">
-        <v>0.74</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -547,24 +547,24 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>05-17</t>
+          <t>06-06</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Near DC</t>
+          <t>Wyoming Plus</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C5" t="n">
-        <v>0.77</v>
+        <v>0.67</v>
       </c>
       <c r="D5" t="n">
-        <v>0.79</v>
+        <v>0.67</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -574,24 +574,24 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>10-24</t>
+          <t>09-29</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Oregon Plus</t>
+          <t>Louisiana Plus</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>177</v>
+        <v>97</v>
       </c>
       <c r="C6" t="n">
-        <v>0.74</v>
+        <v>0.78</v>
       </c>
       <c r="D6" t="n">
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -601,24 +601,24 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>06-26</t>
+          <t>04-07</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Oregon Plus</t>
+          <t>Louisiana Plus</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>272</v>
+        <v>337</v>
       </c>
       <c r="C7" t="n">
-        <v>0.82</v>
+        <v>0.72</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.71</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -628,24 +628,24 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>09-29</t>
+          <t>12-03</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Northeast Plus</t>
+          <t>Alaska State</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>157</v>
+        <v>212</v>
       </c>
       <c r="C8" t="n">
-        <v>0.74</v>
+        <v>0.84</v>
       </c>
       <c r="D8" t="n">
-        <v>0.72</v>
+        <v>0.85</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -655,24 +655,24 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>06-06</t>
+          <t>07-31</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Northeast Plus</t>
+          <t>Alaska State</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>287</v>
+        <v>217</v>
       </c>
       <c r="C9" t="n">
-        <v>0.78</v>
+        <v>0.86</v>
       </c>
       <c r="D9" t="n">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -682,24 +682,24 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>10-14</t>
+          <t>08-05</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Minnesota Plus</t>
+          <t>New Mexico Plus</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>177</v>
+        <v>112</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8</v>
+        <v>0.66</v>
       </c>
       <c r="D10" t="n">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -709,24 +709,24 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>06-26</t>
+          <t>04-22</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Minnesota Plus</t>
+          <t>New Mexico Plus</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>252</v>
+        <v>297</v>
       </c>
       <c r="C11" t="n">
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="D11" t="n">
-        <v>0.77</v>
+        <v>0.64</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -736,24 +736,24 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>09-09</t>
+          <t>10-24</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hawaii State</t>
+          <t>Minnesota Plus</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="C12" t="n">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="D12" t="n">
-        <v>0.79</v>
+        <v>0.78</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -763,24 +763,24 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>02-21</t>
+          <t>06-26</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hawaii State</t>
+          <t>Minnesota Plus</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>365</v>
+        <v>252</v>
       </c>
       <c r="C13" t="n">
-        <v>0.64</v>
+        <v>0.82</v>
       </c>
       <c r="D13" t="n">
-        <v>0.63</v>
+        <v>0.82</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -790,24 +790,24 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>12-31</t>
+          <t>09-09</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Alaska State</t>
+          <t>Indiana Plus</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="C14" t="n">
-        <v>0.85</v>
+        <v>0.79</v>
       </c>
       <c r="D14" t="n">
-        <v>0.88</v>
+        <v>0.76</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -817,24 +817,24 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>07-19</t>
+          <t>06-06</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Alaska State</t>
+          <t>Indiana Plus</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="C15" t="n">
-        <v>0.87</v>
+        <v>0.84</v>
       </c>
       <c r="D15" t="n">
-        <v>0.87</v>
+        <v>0.79</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -844,24 +844,24 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>09-03</t>
+          <t>09-14</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Wyoming Plus</t>
+          <t>Northeast Plus</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>157</v>
       </c>
       <c r="C16" t="n">
-        <v>0.66</v>
+        <v>0.79</v>
       </c>
       <c r="D16" t="n">
-        <v>0.65</v>
+        <v>0.76</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -878,17 +878,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Wyoming Plus</t>
+          <t>Northeast Plus</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C17" t="n">
-        <v>0.61</v>
+        <v>0.79</v>
       </c>
       <c r="D17" t="n">
-        <v>0.62</v>
+        <v>0.8</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -898,7 +898,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>09-29</t>
+          <t>10-04</t>
         </is>
       </c>
     </row>
@@ -912,10 +912,10 @@
         <v>37</v>
       </c>
       <c r="C18" t="n">
-        <v>0.71</v>
+        <v>0.75</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7</v>
+        <v>0.73</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -939,10 +939,10 @@
         <v>362</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.75</v>
       </c>
       <c r="D19" t="n">
-        <v>0.67</v>
+        <v>0.72</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -966,10 +966,10 @@
         <v>147</v>
       </c>
       <c r="C20" t="n">
-        <v>0.72</v>
+        <v>0.76</v>
       </c>
       <c r="D20" t="n">
-        <v>0.72</v>
+        <v>0.76</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -993,10 +993,10 @@
         <v>282</v>
       </c>
       <c r="C21" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D21" t="n">
         <v>0.74</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.6899999999999999</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -1013,17 +1013,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Puerto Rico</t>
+          <t>Georgia Plus</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1</v>
+        <v>0.83</v>
       </c>
       <c r="D22" t="n">
-        <v>0.08</v>
+        <v>0.79</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1033,24 +1033,24 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>03-08</t>
+          <t>04-27</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Puerto Rico</t>
+          <t>Georgia Plus</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>365</v>
+        <v>302</v>
       </c>
       <c r="C23" t="n">
-        <v>0.05</v>
+        <v>0.79</v>
       </c>
       <c r="D23" t="n">
-        <v>0.02</v>
+        <v>0.79</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -1060,24 +1060,24 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>12-31</t>
+          <t>10-29</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>East Canada</t>
+          <t>Hawaii State</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>182</v>
+        <v>72</v>
       </c>
       <c r="C24" t="n">
-        <v>0.77</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D24" t="n">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1087,24 +1087,24 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>07-01</t>
+          <t>03-13</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>East Canada</t>
+          <t>Hawaii State</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>257</v>
+        <v>365</v>
       </c>
       <c r="C25" t="n">
-        <v>0.78</v>
+        <v>0.67</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -1114,24 +1114,24 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>09-14</t>
+          <t>12-31</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>California Plus</t>
+          <t>Near DC</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C26" t="n">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
       <c r="D26" t="n">
-        <v>0.73</v>
+        <v>0.78</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1141,24 +1141,24 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>05-22</t>
+          <t>05-17</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>California Plus</t>
+          <t>Near DC</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="C27" t="n">
-        <v>0.71</v>
+        <v>0.8</v>
       </c>
       <c r="D27" t="n">
-        <v>0.73</v>
+        <v>0.82</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -1168,24 +1168,24 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>11-08</t>
+          <t>10-24</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Georgia Plus</t>
+          <t>Oregon Plus</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>117</v>
+        <v>177</v>
       </c>
       <c r="C28" t="n">
         <v>0.78</v>
       </c>
       <c r="D28" t="n">
-        <v>0.75</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -1195,24 +1195,24 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>04-27</t>
+          <t>06-26</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Georgia Plus</t>
+          <t>Oregon Plus</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>302</v>
+        <v>267</v>
       </c>
       <c r="C29" t="n">
-        <v>0.74</v>
+        <v>0.82</v>
       </c>
       <c r="D29" t="n">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="E29" t="n">
         <v>1</v>
@@ -1222,24 +1222,24 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>10-29</t>
+          <t>09-24</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Indiana Plus</t>
+          <t>Puerto Rico</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>157</v>
+        <v>32</v>
       </c>
       <c r="C30" t="n">
-        <v>0.76</v>
+        <v>0.14</v>
       </c>
       <c r="D30" t="n">
-        <v>0.72</v>
+        <v>0.2</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -1249,24 +1249,24 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>06-06</t>
+          <t>02-01</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Indiana Plus</t>
+          <t>Puerto Rico</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>262</v>
+        <v>365</v>
       </c>
       <c r="C31" t="n">
-        <v>0.73</v>
+        <v>0.13</v>
       </c>
       <c r="D31" t="n">
-        <v>0.75</v>
+        <v>0.1</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
@@ -1276,24 +1276,24 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>09-19</t>
+          <t>12-31</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>New Mexico Plus</t>
+          <t>California Plus</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="C32" t="n">
-        <v>0.59</v>
+        <v>0.77</v>
       </c>
       <c r="D32" t="n">
-        <v>0.6</v>
+        <v>0.79</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1303,24 +1303,24 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>04-17</t>
+          <t>05-27</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>New Mexico Plus</t>
+          <t>California Plus</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="C33" t="n">
-        <v>0.6</v>
+        <v>0.76</v>
       </c>
       <c r="D33" t="n">
-        <v>0.59</v>
+        <v>0.76</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
@@ -1330,7 +1330,34 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>10-24</t>
+          <t>11-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>California Plus</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>312</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>11-08</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish testing (completes rough draft)
</commit_message>
<xml_diff>
--- a/C_Output/best_month_for_route.xlsx
+++ b/C_Output/best_month_for_route.xlsx
@@ -473,17 +473,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>East Canada</t>
+          <t>Louisiana Plus</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>177</v>
+        <v>97</v>
       </c>
       <c r="C2" t="n">
-        <v>0.84</v>
+        <v>0.78</v>
       </c>
       <c r="D2" t="n">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -493,24 +493,24 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>06-26</t>
+          <t>04-07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>East Canada</t>
+          <t>Louisiana Plus</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>257</v>
+        <v>337</v>
       </c>
       <c r="C3" t="n">
-        <v>0.86</v>
+        <v>0.72</v>
       </c>
       <c r="D3" t="n">
-        <v>0.86</v>
+        <v>0.71</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -520,24 +520,24 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>09-14</t>
+          <t>12-03</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Wyoming Plus</t>
+          <t>East Canada</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C4" t="n">
-        <v>0.71</v>
+        <v>0.84</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.82</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -547,24 +547,24 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>06-06</t>
+          <t>06-26</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Wyoming Plus</t>
+          <t>East Canada</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="C5" t="n">
-        <v>0.67</v>
+        <v>0.86</v>
       </c>
       <c r="D5" t="n">
-        <v>0.67</v>
+        <v>0.86</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -574,21 +574,21 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>09-29</t>
+          <t>09-14</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Louisiana Plus</t>
+          <t>Northeast Plus</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>97</v>
+        <v>157</v>
       </c>
       <c r="C6" t="n">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="D6" t="n">
         <v>0.76</v>
@@ -601,24 +601,24 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>04-07</t>
+          <t>06-06</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Louisiana Plus</t>
+          <t>Northeast Plus</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>337</v>
+        <v>277</v>
       </c>
       <c r="C7" t="n">
-        <v>0.72</v>
+        <v>0.79</v>
       </c>
       <c r="D7" t="n">
-        <v>0.71</v>
+        <v>0.8</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -628,24 +628,24 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>12-03</t>
+          <t>10-04</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Alaska State</t>
+          <t>Missouri Plus</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>212</v>
+        <v>147</v>
       </c>
       <c r="C8" t="n">
-        <v>0.84</v>
+        <v>0.76</v>
       </c>
       <c r="D8" t="n">
-        <v>0.85</v>
+        <v>0.76</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -655,24 +655,24 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>07-31</t>
+          <t>05-27</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Alaska State</t>
+          <t>Missouri Plus</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>217</v>
+        <v>282</v>
       </c>
       <c r="C9" t="n">
-        <v>0.86</v>
+        <v>0.78</v>
       </c>
       <c r="D9" t="n">
-        <v>0.85</v>
+        <v>0.74</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -682,24 +682,24 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>08-05</t>
+          <t>10-09</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>New Mexico Plus</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="C10" t="n">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="D10" t="n">
-        <v>0.65</v>
+        <v>0.73</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -709,24 +709,24 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>04-22</t>
+          <t>02-06</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>New Mexico Plus</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>297</v>
+        <v>362</v>
       </c>
       <c r="C11" t="n">
-        <v>0.63</v>
+        <v>0.75</v>
       </c>
       <c r="D11" t="n">
-        <v>0.64</v>
+        <v>0.72</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -736,25 +736,25 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>10-24</t>
+          <t>12-28</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Minnesota Plus</t>
+          <t>Alaska State</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>177</v>
+        <v>212</v>
       </c>
       <c r="C12" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.85</v>
       </c>
-      <c r="D12" t="n">
-        <v>0.78</v>
-      </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
@@ -763,24 +763,24 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>06-26</t>
+          <t>07-31</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Minnesota Plus</t>
+          <t>Alaska State</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="C13" t="n">
-        <v>0.82</v>
+        <v>0.86</v>
       </c>
       <c r="D13" t="n">
-        <v>0.82</v>
+        <v>0.85</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -790,24 +790,24 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>09-09</t>
+          <t>08-05</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Indiana Plus</t>
+          <t>Near DC</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="C14" t="n">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="D14" t="n">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -817,24 +817,24 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>06-06</t>
+          <t>05-17</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Indiana Plus</t>
+          <t>Near DC</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>257</v>
+        <v>297</v>
       </c>
       <c r="C15" t="n">
-        <v>0.84</v>
+        <v>0.8</v>
       </c>
       <c r="D15" t="n">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -844,24 +844,24 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>09-14</t>
+          <t>10-24</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Northeast Plus</t>
+          <t>Minnesota Plus</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C16" t="n">
-        <v>0.79</v>
+        <v>0.85</v>
       </c>
       <c r="D16" t="n">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -871,24 +871,24 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>06-06</t>
+          <t>06-26</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Northeast Plus</t>
+          <t>Minnesota Plus</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="C17" t="n">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -898,24 +898,24 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>10-04</t>
+          <t>09-09</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Georgia Plus</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>37</v>
+        <v>117</v>
       </c>
       <c r="C18" t="n">
-        <v>0.75</v>
+        <v>0.83</v>
       </c>
       <c r="D18" t="n">
-        <v>0.73</v>
+        <v>0.79</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -925,24 +925,24 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>02-06</t>
+          <t>04-27</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>Georgia Plus</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>362</v>
+        <v>302</v>
       </c>
       <c r="C19" t="n">
-        <v>0.75</v>
+        <v>0.79</v>
       </c>
       <c r="D19" t="n">
-        <v>0.72</v>
+        <v>0.79</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -952,21 +952,21 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>12-28</t>
+          <t>10-29</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Missouri Plus</t>
+          <t>Indiana Plus</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C20" t="n">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="D20" t="n">
         <v>0.76</v>
@@ -979,24 +979,24 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>05-27</t>
+          <t>06-06</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Missouri Plus</t>
+          <t>Indiana Plus</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="C21" t="n">
-        <v>0.78</v>
+        <v>0.84</v>
       </c>
       <c r="D21" t="n">
-        <v>0.74</v>
+        <v>0.79</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -1006,24 +1006,24 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>10-09</t>
+          <t>09-14</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Georgia Plus</t>
+          <t>New Mexico Plus</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C22" t="n">
-        <v>0.83</v>
+        <v>0.66</v>
       </c>
       <c r="D22" t="n">
-        <v>0.79</v>
+        <v>0.65</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1033,24 +1033,24 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>04-27</t>
+          <t>04-22</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Georgia Plus</t>
+          <t>New Mexico Plus</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C23" t="n">
-        <v>0.79</v>
+        <v>0.63</v>
       </c>
       <c r="D23" t="n">
-        <v>0.79</v>
+        <v>0.64</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -1060,25 +1060,25 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>10-29</t>
+          <t>10-24</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Hawaii State</t>
+          <t>Oregon Plus</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>72</v>
+        <v>177</v>
       </c>
       <c r="C24" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D24" t="n">
         <v>0.8100000000000001</v>
       </c>
-      <c r="D24" t="n">
-        <v>0.83</v>
-      </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
@@ -1087,24 +1087,24 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>03-13</t>
+          <t>06-26</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Hawaii State</t>
+          <t>Oregon Plus</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>365</v>
+        <v>267</v>
       </c>
       <c r="C25" t="n">
-        <v>0.67</v>
+        <v>0.82</v>
       </c>
       <c r="D25" t="n">
-        <v>0.67</v>
+        <v>0.85</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -1114,24 +1114,24 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>12-31</t>
+          <t>09-24</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Near DC</t>
+          <t>California Plus</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C26" t="n">
         <v>0.77</v>
       </c>
       <c r="D26" t="n">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1141,24 +1141,24 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>05-17</t>
+          <t>05-27</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Near DC</t>
+          <t>California Plus</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8</v>
+        <v>0.76</v>
       </c>
       <c r="D27" t="n">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -1168,186 +1168,186 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>10-24</t>
+          <t>11-07</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Oregon Plus</t>
+          <t>California Plus</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>177</v>
+        <v>312</v>
       </c>
       <c r="C28" t="n">
-        <v>0.78</v>
+        <v>0.76</v>
       </c>
       <c r="D28" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>06-26</t>
+          <t>11-08</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Oregon Plus</t>
+          <t>Hawaii State</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>267</v>
+        <v>72</v>
       </c>
       <c r="C29" t="n">
-        <v>0.82</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D29" t="n">
-        <v>0.85</v>
+        <v>0.83</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>09-24</t>
+          <t>03-13</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Puerto Rico</t>
+          <t>Hawaii State</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>32</v>
+        <v>365</v>
       </c>
       <c r="C30" t="n">
-        <v>0.14</v>
+        <v>0.67</v>
       </c>
       <c r="D30" t="n">
-        <v>0.2</v>
+        <v>0.67</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>02-01</t>
+          <t>12-31</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Puerto Rico</t>
+          <t>Wyoming Plus</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>365</v>
+        <v>157</v>
       </c>
       <c r="C31" t="n">
-        <v>0.13</v>
+        <v>0.71</v>
       </c>
       <c r="D31" t="n">
-        <v>0.1</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="b">
         <v>1</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>12-31</t>
+          <t>06-06</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>California Plus</t>
+          <t>Wyoming Plus</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>147</v>
+        <v>272</v>
       </c>
       <c r="C32" t="n">
-        <v>0.77</v>
+        <v>0.67</v>
       </c>
       <c r="D32" t="n">
-        <v>0.79</v>
+        <v>0.67</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="b">
         <v>1</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>05-27</t>
+          <t>09-29</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>California Plus</t>
+          <t>Puerto Rico</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>311</v>
+        <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.76</v>
+        <v>0.14</v>
       </c>
       <c r="D33" t="n">
-        <v>0.76</v>
+        <v>0.2</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="b">
         <v>1</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>11-07</t>
+          <t>02-01</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>California Plus</t>
+          <t>Puerto Rico</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>312</v>
+        <v>365</v>
       </c>
       <c r="C34" t="n">
-        <v>0.76</v>
+        <v>0.13</v>
       </c>
       <c r="D34" t="n">
-        <v>0.76</v>
+        <v>0.1</v>
       </c>
       <c r="E34" t="n">
         <v>1</v>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>11-08</t>
+          <t>12-31</t>
         </is>
       </c>
     </row>

</xml_diff>